<commit_message>
Updated RAD Summary Test Data.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/Summary.xlsx
+++ b/KatalonData/RADTestData/Summary.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{15A710D7-B11D-4289-A2D1-FF452E6A6C2B}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6D1F86-E0C9-40DB-9D59-34527CD0A185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="7" windowHeight="14010" windowWidth="24525" xWindow="1680" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="2580"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="7" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Estimated" r:id="rId1" sheetId="1"/>
-    <sheet name="Existing" r:id="rId2" sheetId="2"/>
-    <sheet name="Extension" r:id="rId3" sheetId="3"/>
-    <sheet name="NewTaxReturn" r:id="rId4" sheetId="4"/>
-    <sheet name="Personal" r:id="rId5" sheetId="5"/>
-    <sheet name="Personal_IND" r:id="rId6" sheetId="6"/>
-    <sheet name="Personal_JNT" r:id="rId7" sheetId="7"/>
-    <sheet name="Personal_EL" r:id="rId8" sheetId="8"/>
+    <sheet name="Estimated" sheetId="1" r:id="rId1"/>
+    <sheet name="Existing" sheetId="2" r:id="rId2"/>
+    <sheet name="Extension" sheetId="3" r:id="rId3"/>
+    <sheet name="NewTaxReturn" sheetId="4" r:id="rId4"/>
+    <sheet name="Personal" sheetId="5" r:id="rId5"/>
+    <sheet name="Personal_IND" sheetId="6" r:id="rId6"/>
+    <sheet name="Personal_JNT" sheetId="7" r:id="rId7"/>
+    <sheet name="Personal_EL" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="142">
   <si>
     <t>Result</t>
   </si>
@@ -234,213 +234,6 @@
     <t>Thu Jan 25 17:51:54 EST 2024</t>
   </si>
   <si>
-    <t>Thu Jan 25 17:52:30 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 17:53:09 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 17:53:47 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 17:54:25 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 17:55:04 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 17:55:43 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 17:56:23 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 17:57:03 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 17:57:41 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 17:58:21 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 17:58:59 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 17:59:36 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:01:28 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:02:06 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:02:43 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:03:20 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:03:57 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:04:35 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:05:15 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:05:51 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:06:27 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:07:04 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:07:41 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:08:17 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:08:54 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:09:30 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:10:07 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:10:44 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:11:20 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:11:57 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:12:34 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:13:12 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:13:49 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:14:25 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:15:02 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:15:38 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:16:15 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:18:04 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:18:40 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:19:17 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:19:53 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:20:30 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:21:07 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:21:43 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:22:20 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:22:56 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:23:32 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:24:09 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:24:46 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:26:38 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:27:15 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:27:51 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:28:28 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:29:04 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:29:41 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:30:17 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:30:54 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:31:29 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:32:06 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:32:42 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:33:18 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:35:06 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:35:44 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:36:20 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:36:57 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:37:34 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:38:10 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:38:47 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:39:24 EST 2024</t>
-  </si>
-  <si>
     <t>Thu Jan 25 18:40:36 EST 2024</t>
   </si>
   <si>
@@ -465,15 +258,9 @@
     <t>Thu Jan 25 18:44:51 EST 2024</t>
   </si>
   <si>
-    <t>Thu Jan 25 22:21:13 EST 2024</t>
-  </si>
-  <si>
     <t>Thu Jan 25 22:21:51 EST 2024</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Thu Jan 25 22:47:17 EST 2024</t>
   </si>
   <si>
@@ -679,13 +466,15 @@
   </si>
   <si>
     <t>Thu Jan 25 23:29:53 EST 2024</t>
+  </si>
+  <si>
+    <t>Mon Jan 29 12:02:47 EST 2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -728,19 +517,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -757,10 +546,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -795,7 +584,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -847,7 +636,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -958,21 +747,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -989,7 +778,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1041,15 +830,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
-  <dimension ref="A1:I7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
@@ -1057,15 +846,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="44.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="35.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="19.5703125" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
+    <col min="4" max="4" width="44.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1245,8 +1034,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1254,8 +1043,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
-  <dimension ref="A1:G19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14:XFD14"/>
@@ -1263,12 +1052,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="37.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
+    <col min="4" max="4" width="37.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1296,7 +1085,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>72</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1313,7 +1102,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>73</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1330,7 +1119,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1347,7 +1136,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>75</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1367,7 +1156,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>147</v>
+        <v>76</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1387,7 +1176,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>148</v>
+        <v>77</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1404,7 +1193,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>149</v>
+        <v>78</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -1421,7 +1210,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>150</v>
+        <v>79</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -1438,7 +1227,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>80</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -1455,7 +1244,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>152</v>
+        <v>81</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -1475,7 +1264,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -1495,7 +1284,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>154</v>
+        <v>83</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -1512,7 +1301,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>155</v>
+        <v>84</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -1529,7 +1318,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>156</v>
+        <v>85</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -1546,7 +1335,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>157</v>
+        <v>86</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -1566,7 +1355,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>158</v>
+        <v>87</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -1583,7 +1372,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>159</v>
+        <v>88</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -1600,7 +1389,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>160</v>
+        <v>89</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -1613,7 +1402,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1621,8 +1410,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
-  <dimension ref="A1:I7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C7"/>
@@ -1630,15 +1419,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="35.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="24.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="27.0" collapsed="true"/>
-    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="17.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="35" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="7" width="17" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1803,7 +1592,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1811,23 +1600,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
-  <dimension ref="A1:H52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="A45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="30.28515625" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="31.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="38.7109375" collapsed="true"/>
-    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
-    <col min="8" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="30.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
+    <col min="4" max="4" width="31.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="38.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="7" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1858,7 +1647,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>90</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1878,7 +1667,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>91</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1901,7 +1690,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>92</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1924,7 +1713,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>93</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1947,7 +1736,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>165</v>
+        <v>94</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1970,7 +1759,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>166</v>
+        <v>95</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1990,7 +1779,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>167</v>
+        <v>96</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -2013,7 +1802,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>168</v>
+        <v>97</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -2036,7 +1825,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>169</v>
+        <v>98</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -2059,7 +1848,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>170</v>
+        <v>99</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -2082,7 +1871,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>171</v>
+        <v>100</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2102,7 +1891,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>172</v>
+        <v>101</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -2125,7 +1914,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>173</v>
+        <v>102</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -2148,7 +1937,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>174</v>
+        <v>103</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -2171,7 +1960,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>175</v>
+        <v>104</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -2194,7 +1983,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2214,7 +2003,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>177</v>
+        <v>106</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -2234,7 +2023,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>178</v>
+        <v>107</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2254,7 +2043,7 @@
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>179</v>
+        <v>108</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
@@ -2274,7 +2063,7 @@
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>180</v>
+        <v>109</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
@@ -2294,7 +2083,7 @@
         <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>181</v>
+        <v>110</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -2314,7 +2103,7 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>182</v>
+        <v>111</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -2334,7 +2123,7 @@
         <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>183</v>
+        <v>112</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -2354,7 +2143,7 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>184</v>
+        <v>113</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>32</v>
@@ -2377,7 +2166,7 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>185</v>
+        <v>114</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -2397,7 +2186,7 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>186</v>
+        <v>115</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
@@ -2417,7 +2206,7 @@
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>187</v>
+        <v>116</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -2437,7 +2226,7 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>188</v>
+        <v>117</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
@@ -2457,7 +2246,7 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>189</v>
+        <v>118</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>32</v>
@@ -2477,7 +2266,7 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>190</v>
+        <v>119</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>32</v>
@@ -2497,7 +2286,7 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>191</v>
+        <v>120</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>32</v>
@@ -2517,7 +2306,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>32</v>
@@ -2537,7 +2326,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>32</v>
@@ -2557,7 +2346,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>194</v>
+        <v>123</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>32</v>
@@ -2577,7 +2366,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>195</v>
+        <v>124</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>32</v>
@@ -2597,7 +2386,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>196</v>
+        <v>125</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>32</v>
@@ -2620,7 +2409,7 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>197</v>
+        <v>126</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>32</v>
@@ -2640,7 +2429,7 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>198</v>
+        <v>127</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>32</v>
@@ -2660,7 +2449,7 @@
         <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>199</v>
+        <v>128</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
@@ -2680,7 +2469,7 @@
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>200</v>
+        <v>129</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>32</v>
@@ -2700,7 +2489,7 @@
         <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>201</v>
+        <v>130</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>32</v>
@@ -2720,7 +2509,7 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>202</v>
+        <v>131</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>32</v>
@@ -2740,7 +2529,7 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>203</v>
+        <v>132</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>32</v>
@@ -2760,7 +2549,7 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>204</v>
+        <v>133</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>32</v>
@@ -2780,7 +2569,7 @@
         <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>205</v>
+        <v>134</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
@@ -2800,7 +2589,7 @@
         <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>206</v>
+        <v>135</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>32</v>
@@ -2820,7 +2609,7 @@
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>207</v>
+        <v>136</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>32</v>
@@ -2840,7 +2629,7 @@
         <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>208</v>
+        <v>137</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>32</v>
@@ -2863,7 +2652,7 @@
         <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>209</v>
+        <v>138</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>32</v>
@@ -2883,7 +2672,7 @@
         <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>210</v>
+        <v>139</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>32</v>
@@ -2903,7 +2692,7 @@
         <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>211</v>
+        <v>140</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>32</v>
@@ -2919,8 +2708,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2928,8 +2717,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4:F7"/>
@@ -2937,15 +2726,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="23.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3032,7 +2821,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3040,8 +2829,184 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
-  <dimension ref="A1:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="26.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7:C9"/>
@@ -3049,12 +3014,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="14.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3082,7 +3047,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>67</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3102,7 +3067,7 @@
         <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>46</v>
@@ -3122,7 +3087,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>68</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3142,7 +3107,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>69</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3162,7 +3127,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>70</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3211,189 +3176,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
-  <dimension ref="A1:G9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="17.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>139</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -3401,12 +3190,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.0" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="26" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3431,7 +3220,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3448,7 +3237,7 @@
         <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>71</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>14</v>
@@ -3458,6 +3247,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>